<commit_message>
feat: added new organisations and image paths
</commit_message>
<xml_diff>
--- a/erns/cranio/cranio_emx2.xlsx
+++ b/erns/cranio/cranio_emx2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-erns/erns/cranio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795CA90A-A45E-E44C-95AE-573325C4F639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFDD231-1A3C-4041-996A-D62AA0EDB78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17500" activeTab="3" xr2:uid="{3D9FBA9F-6CBA-0544-BBF9-FE715A841ECF}"/>
+    <workbookView xWindow="-33060" yWindow="-1820" windowWidth="29400" windowHeight="17500" activeTab="4" xr2:uid="{3D9FBA9F-6CBA-0544-BBF9-FE715A841ECF}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="statistics" sheetId="3" r:id="rId4"/>
     <sheet name="dataproviders" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -525,18 +525,9 @@
     <t>description</t>
   </si>
   <si>
-    <t>David</t>
-  </si>
-  <si>
     <t>definition</t>
   </si>
   <si>
-    <t>live</t>
-  </si>
-  <si>
-    <t>David2</t>
-  </si>
-  <si>
     <t>imageUrl</t>
   </si>
   <si>
@@ -544,6 +535,57 @@
   </si>
   <si>
     <t>profiles/erasmus-mc.jpg</t>
+  </si>
+  <si>
+    <t>profiles/umc-utrecht.jpg</t>
+  </si>
+  <si>
+    <t>profiles/fondazione-a-gemelli.jpg</t>
+  </si>
+  <si>
+    <t>profiles/universitatsklinikum-charite.jpg</t>
+  </si>
+  <si>
+    <t>Szent-Gyorgyi Albert Medical Center</t>
+  </si>
+  <si>
+    <t>profiles/szent-medical-center.jpg</t>
+  </si>
+  <si>
+    <t>https://ror.org/01pnej532</t>
+  </si>
+  <si>
+    <t>01pnej532</t>
+  </si>
+  <si>
+    <t>Szeged</t>
+  </si>
+  <si>
+    <t>HU2</t>
+  </si>
+  <si>
+    <t>UZ Leuven</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>profiles/uz-leuven.jpg</t>
+  </si>
+  <si>
+    <t>https://ror.org/0424bsv16</t>
+  </si>
+  <si>
+    <t>0424bsv16</t>
+  </si>
+  <si>
+    <t>Leuven</t>
+  </si>
+  <si>
+    <t>profiles/ospedale-san-gerardo-monza.jpg</t>
+  </si>
+  <si>
+    <t>BE1</t>
   </si>
 </sst>
 </file>
@@ -566,12 +608,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -586,9 +634,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,7 +986,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,27 +1002,14 @@
         <v>108</v>
       </c>
       <c r="C1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>163</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -981,16 +1018,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0060A8-8459-FC44-9EF8-4FF513B74D7E}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1019,400 +1057,413 @@
         <v>75</v>
       </c>
       <c r="I1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2">
-        <v>48.583919999999999</v>
-      </c>
-      <c r="H2">
-        <v>7.7455299999999996</v>
+      <c r="A2" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="3">
+        <v>50.87959</v>
+      </c>
+      <c r="H2" s="3">
+        <v>4.7009299999999996</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3">
-        <v>57.707160000000002</v>
-      </c>
-      <c r="H3">
-        <v>11.96679</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="3">
+        <v>50.072868999999997</v>
+      </c>
+      <c r="H3" s="3">
+        <v>14.340355000000001</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="G4">
-        <v>40.416499999999999</v>
+        <v>60.188611000000002</v>
       </c>
       <c r="H4">
-        <v>-3.7025600000000001</v>
+        <v>24.905277999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G5">
-        <v>41.428083000000001</v>
+        <v>50.63297</v>
       </c>
       <c r="H5">
-        <v>2.1422780000000001</v>
+        <v>3.0585800000000001</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G6">
-        <v>59.32938</v>
+        <v>48.853409999999997</v>
       </c>
       <c r="H6">
-        <v>18.068709999999999</v>
-      </c>
-      <c r="I6" t="s">
-        <v>166</v>
+        <v>2.3488000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G7">
-        <v>51.842500000000001</v>
+        <v>48.583919999999999</v>
       </c>
       <c r="H7">
-        <v>5.8527800000000001</v>
+        <v>7.7455299999999996</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8">
-        <v>52.090829999999997</v>
-      </c>
-      <c r="H8">
-        <v>5.1222200000000004</v>
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="3">
+        <v>52.524369999999998</v>
+      </c>
+      <c r="H8" s="3">
+        <v>13.41053</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9">
-        <v>48.853409999999997</v>
-      </c>
-      <c r="H9">
-        <v>2.3488000000000002</v>
+      <c r="A9" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="3">
+        <v>46.253</v>
+      </c>
+      <c r="H9" s="3">
+        <v>20.148240000000001</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="G10">
-        <v>50.63297</v>
+        <v>46.072499999999998</v>
       </c>
       <c r="H10">
-        <v>3.0585800000000001</v>
+        <v>18.230830000000001</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
         <v>90</v>
       </c>
       <c r="G11">
+        <v>45.404313999999999</v>
+      </c>
+      <c r="H11">
+        <v>11.887473999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="3">
         <v>41.891930000000002</v>
       </c>
-      <c r="H11">
+      <c r="H12" s="3">
         <v>12.511329999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12">
-        <v>52.524369999999998</v>
-      </c>
-      <c r="H12">
-        <v>13.41053</v>
+      <c r="I12" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G13">
-        <v>59.847222000000002</v>
+        <v>45.477186000000003</v>
       </c>
       <c r="H13">
-        <v>17.640277999999999</v>
+        <v>9.2303850000000001</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G14">
-        <v>45.477186000000003</v>
-      </c>
-      <c r="H14">
-        <v>9.2303850000000001</v>
+      <c r="G14" s="3">
+        <v>45.603031000000001</v>
+      </c>
+      <c r="H14" s="3">
+        <v>9.2587820000000001</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G15">
-        <v>46.072499999999998</v>
+        <v>45.555954</v>
       </c>
       <c r="H15">
-        <v>18.230830000000001</v>
+        <v>11.546531999999999</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
         <v>90</v>
       </c>
       <c r="G16">
-        <v>45.404313999999999</v>
+        <v>45.434807999999997</v>
       </c>
       <c r="H16">
-        <v>11.887473999999999</v>
+        <v>9.1598159999999993</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1441,166 +1492,228 @@
         <v>4.4791699999999999</v>
       </c>
       <c r="I17" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G18">
-        <v>45.434807999999997</v>
+        <v>51.842500000000001</v>
       </c>
       <c r="H18">
-        <v>9.1598159999999993</v>
+        <v>5.8527800000000001</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" t="s">
-        <v>100</v>
-      </c>
-      <c r="G19">
-        <v>38.748764000000001</v>
-      </c>
-      <c r="H19">
-        <v>-9.1607160000000007</v>
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="3">
+        <v>52.090829999999997</v>
+      </c>
+      <c r="H19" s="3">
+        <v>5.1222200000000004</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G20">
-        <v>50.072868999999997</v>
+        <v>38.748764000000001</v>
       </c>
       <c r="H20">
-        <v>14.340355000000001</v>
+        <v>-9.1607160000000007</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G21">
-        <v>45.603031000000001</v>
+        <v>40.416499999999999</v>
       </c>
       <c r="H21">
-        <v>9.2587820000000001</v>
+        <v>-3.7025600000000001</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="G22">
-        <v>60.188611000000002</v>
+        <v>41.428083000000001</v>
       </c>
       <c r="H22">
-        <v>24.905277999999999</v>
+        <v>2.1422780000000001</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="F23" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G23">
-        <v>45.555954</v>
+        <v>59.32938</v>
       </c>
       <c r="H23">
-        <v>11.546531999999999</v>
+        <v>18.068709999999999</v>
+      </c>
+      <c r="I23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24">
+        <v>57.707160000000002</v>
+      </c>
+      <c r="H24">
+        <v>11.96679</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25">
+        <v>59.847222000000002</v>
+      </c>
+      <c r="H25">
+        <v>17.640277999999999</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I25">
+    <sortCondition ref="F2:F25"/>
+    <sortCondition ref="A2:A25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1609,7 +1722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB669A98-DA48-D54D-A256-485349776BE1}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+    <sheetView zoomScale="104" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1802,10 +1915,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6366C3-CBA3-F348-A0A6-D45D62B83798}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1982,10 +2095,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -1993,10 +2106,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -2004,10 +2117,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -2015,10 +2128,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -2026,10 +2139,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -2037,10 +2150,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -2048,10 +2161,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -2059,12 +2172,34 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>131</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="b">
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: added schema settings
</commit_message>
<xml_diff>
--- a/erns/cranio/cranio_emx2.xlsx
+++ b/erns/cranio/cranio_emx2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-erns/erns/cranio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFDD231-1A3C-4041-996A-D62AA0EDB78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E614FC-5D84-614B-AAC2-A006681F33C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33060" yWindow="-1820" windowWidth="29400" windowHeight="17500" activeTab="4" xr2:uid="{3D9FBA9F-6CBA-0544-BBF9-FE715A841ECF}"/>
+    <workbookView xWindow="-34300" yWindow="-2400" windowWidth="29400" windowHeight="17500" activeTab="2" xr2:uid="{3D9FBA9F-6CBA-0544-BBF9-FE715A841ECF}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="184">
   <si>
     <t>name</t>
   </si>
@@ -586,6 +586,12 @@
   </si>
   <si>
     <t>BE1</t>
+  </si>
+  <si>
+    <t>hasSchema</t>
+  </si>
+  <si>
+    <t>schemaName</t>
   </si>
 </sst>
 </file>
@@ -1018,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0060A8-8459-FC44-9EF8-4FF513B74D7E}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1031,7 +1037,7 @@
     <col min="9" max="9" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1059,8 +1065,14 @@
       <c r="I1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>174</v>
       </c>
@@ -1088,8 +1100,14 @@
       <c r="I2" s="3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1115,8 +1133,14 @@
         <v>14.340355000000001</v>
       </c>
       <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1142,7 +1166,7 @@
         <v>24.905277999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1168,7 +1192,7 @@
         <v>3.0585800000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1218,7 @@
         <v>2.3488000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1220,7 +1244,7 @@
         <v>7.7455299999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1248,8 +1272,14 @@
       <c r="I8" s="3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>168</v>
       </c>
@@ -1277,8 +1307,14 @@
       <c r="I9" s="3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1304,7 +1340,7 @@
         <v>18.230830000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1330,7 +1366,7 @@
         <v>11.887473999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1358,8 +1394,14 @@
       <c r="I12" s="3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1385,7 +1427,7 @@
         <v>9.2303850000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1413,8 +1455,14 @@
       <c r="I14" s="3" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1440,7 +1488,7 @@
         <v>11.546531999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1466,7 +1514,7 @@
         <v>9.1598159999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1494,8 +1542,11 @@
       <c r="I17" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1521,7 +1572,7 @@
         <v>5.8527800000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1549,8 +1600,14 @@
       <c r="I19" s="3" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1576,7 +1633,7 @@
         <v>-9.1607160000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -1602,7 +1659,7 @@
         <v>-3.7025600000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1628,7 +1685,7 @@
         <v>2.1422780000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1656,8 +1713,11 @@
       <c r="I23" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1683,7 +1743,7 @@
         <v>11.96679</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -1917,7 +1977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6366C3-CBA3-F348-A0A6-D45D62B83798}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: updated setup script; edited test dataset
</commit_message>
<xml_diff>
--- a/erns/cranio/cranio_emx2.xlsx
+++ b/erns/cranio/cranio_emx2.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-erns/erns/cranio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E614FC-5D84-614B-AAC2-A006681F33C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A63499A-4BA0-9A47-9056-A4B8ABC1DA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34300" yWindow="-2400" windowWidth="29400" windowHeight="17500" activeTab="2" xr2:uid="{3D9FBA9F-6CBA-0544-BBF9-FE715A841ECF}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="4" r:id="rId1"/>
-    <sheet name="users" sheetId="5" r:id="rId2"/>
-    <sheet name="organisations" sheetId="1" r:id="rId3"/>
-    <sheet name="statistics" sheetId="3" r:id="rId4"/>
-    <sheet name="dataproviders" sheetId="2" r:id="rId5"/>
+    <sheet name="organisations" sheetId="1" r:id="rId2"/>
+    <sheet name="statistics" sheetId="3" r:id="rId3"/>
+    <sheet name="dataproviders" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="183">
   <si>
     <t>name</t>
   </si>
@@ -523,9 +522,6 @@
   </si>
   <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>definition</t>
   </si>
   <si>
     <t>imageUrl</t>
@@ -988,46 +984,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A325068-1830-5B4F-85AE-20E6C13693C4}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0060A8-8459-FC44-9EF8-4FF513B74D7E}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1063,33 +1024,33 @@
         <v>75</v>
       </c>
       <c r="I1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K1" t="s">
         <v>182</v>
-      </c>
-      <c r="K1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="G2" s="3">
         <v>50.87959</v>
@@ -1098,13 +1059,13 @@
         <v>4.7009299999999996</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1270,7 +1231,7 @@
         <v>13.41053</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
@@ -1281,19 +1242,19 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>96</v>
@@ -1305,13 +1266,13 @@
         <v>20.148240000000001</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1392,7 +1353,7 @@
         <v>12.511329999999999</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>
@@ -1453,7 +1414,7 @@
         <v>9.2587820000000001</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
@@ -1515,32 +1476,35 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>51.922499999999999</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>4.4791699999999999</v>
       </c>
-      <c r="I17" t="s">
-        <v>164</v>
+      <c r="I17" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
       </c>
       <c r="K17" t="s">
         <v>125</v>
@@ -1598,7 +1562,7 @@
         <v>5.1222200000000004</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J19" t="b">
         <v>1</v>
@@ -1711,7 +1675,7 @@
         <v>18.068709999999999</v>
       </c>
       <c r="I23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K23" t="s">
         <v>114</v>
@@ -1778,11 +1742,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB669A98-DA48-D54D-A256-485349776BE1}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1973,7 +1937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6366C3-CBA3-F348-A0A6-D45D62B83798}">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -2155,10 +2119,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -2254,10 +2218,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
feat: added py script to prep organisations list
</commit_message>
<xml_diff>
--- a/erns/cranio/cranio_emx2.xlsx
+++ b/erns/cranio/cranio_emx2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-erns/erns/cranio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE3FD76-72AC-C849-BB77-7CE2D8EEEE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE000C61-32BA-D743-9F8B-B5F2B1C74181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3180" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{3D9FBA9F-6CBA-0544-BBF9-FE715A841ECF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="283">
   <si>
     <t>name</t>
   </si>
@@ -885,6 +885,9 @@
   </si>
   <si>
     <t>profiles/vilnius-university-hospital.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fondazione Istituto Neurologico C.Besta </t>
   </si>
 </sst>
 </file>
@@ -940,9 +943,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -980,7 +983,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1086,7 +1089,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1228,7 +1231,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1269,7 +1272,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1926,7 +1929,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>282</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
fixed organisation names; added file paths
</commit_message>
<xml_diff>
--- a/erns/cranio/cranio_emx2.xlsx
+++ b/erns/cranio/cranio_emx2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-erns/erns/cranio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE000C61-32BA-D743-9F8B-B5F2B1C74181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306BC28C-1D5B-4545-B245-5627C77E4D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3180" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{3D9FBA9F-6CBA-0544-BBF9-FE715A841ECF}"/>
+    <workbookView xWindow="-38400" yWindow="-3180" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{3D9FBA9F-6CBA-0544-BBF9-FE715A841ECF}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="325">
   <si>
     <t>name</t>
   </si>
@@ -521,9 +521,6 @@
     <t>organisationType</t>
   </si>
   <si>
-    <t>University Hospital Salzburg, Austria</t>
-  </si>
-  <si>
     <t>05gs8cd61</t>
   </si>
   <si>
@@ -683,9 +680,6 @@
     <t>Florence</t>
   </si>
   <si>
-    <t xml:space="preserve">Fondazione Istituto Neurologico "C.Besta" </t>
-  </si>
-  <si>
     <t xml:space="preserve">Fondazione Policlinico Universitario A. Gemelli </t>
   </si>
   <si>
@@ -833,9 +827,6 @@
     <t>https://ror.org/020sr6z07</t>
   </si>
   <si>
-    <t>University Medical Centre Ljubljana, Slovenia</t>
-  </si>
-  <si>
     <t>01nr6fy72</t>
   </si>
   <si>
@@ -888,6 +879,141 @@
   </si>
   <si>
     <t xml:space="preserve">Fondazione Istituto Neurologico C.Besta </t>
+  </si>
+  <si>
+    <t>imageName</t>
+  </si>
+  <si>
+    <t>university-hospital-salzburg.png</t>
+  </si>
+  <si>
+    <t>hasImage</t>
+  </si>
+  <si>
+    <t>uz-leuven.jpg</t>
+  </si>
+  <si>
+    <t>erasmus-mc.jpg</t>
+  </si>
+  <si>
+    <t>fondazione-a-gemelli.jpg</t>
+  </si>
+  <si>
+    <t>szent-medical-center.jpg</t>
+  </si>
+  <si>
+    <t>umc-utrecht.jpg</t>
+  </si>
+  <si>
+    <t>karolinska-university-hospital.jpg</t>
+  </si>
+  <si>
+    <t>antwerp-university-hospital.jpg</t>
+  </si>
+  <si>
+    <t>University Hospital Salzburg</t>
+  </si>
+  <si>
+    <t>san-gerardo-hospital.jpg</t>
+  </si>
+  <si>
+    <t>uppsal-university-hospital.jpg</t>
+  </si>
+  <si>
+    <t>uz-gent.jpg</t>
+  </si>
+  <si>
+    <t>aarhus-university-hospital.jpg</t>
+  </si>
+  <si>
+    <t>vall-dhebron.jpg</t>
+  </si>
+  <si>
+    <t>university-of-pecs.png</t>
+  </si>
+  <si>
+    <t>university-medical-centre-ljubljana.jpg</t>
+  </si>
+  <si>
+    <t>University Medical Centre Ljubljana</t>
+  </si>
+  <si>
+    <t>vilnius-university-hospital.jpg</t>
+  </si>
+  <si>
+    <t>aop-university-of-padua.jpg</t>
+  </si>
+  <si>
+    <t>aou-meyer-di-firenze.jpg</t>
+  </si>
+  <si>
+    <t>oslo-university-hospital.jpg</t>
+  </si>
+  <si>
+    <t>amsterdam-university-medical-centres.jpg</t>
+  </si>
+  <si>
+    <t>university-hospital-motol.jpg</t>
+  </si>
+  <si>
+    <t>university-hospital-tubingen.jpg</t>
+  </si>
+  <si>
+    <t>smile-house-san-paolo-hospital.jpg</t>
+  </si>
+  <si>
+    <t>san-bortolo-hospital.jpg</t>
+  </si>
+  <si>
+    <t>sahlgrenska-university-hospital.jpg</t>
+  </si>
+  <si>
+    <t>riga-cleft-lip-and-palate-centre-latvia.jpg</t>
+  </si>
+  <si>
+    <t>radboud-mc.jpg</t>
+  </si>
+  <si>
+    <t>hospital-de-sant-joan-de-deu.jpg</t>
+  </si>
+  <si>
+    <t>hospices-civils-de-lyon.jpg</t>
+  </si>
+  <si>
+    <t>hospital-12-de-octubre.jpg</t>
+  </si>
+  <si>
+    <t>mater-dei-hospital.jpg</t>
+  </si>
+  <si>
+    <t>rigshospitalet-copenhagen-university-hospital.jpg</t>
+  </si>
+  <si>
+    <t>regional-specialised-childrens-hospital-olsztyn.jpg</t>
+  </si>
+  <si>
+    <t>fondazione-istituto-neurologico-c-besta.jpg</t>
+  </si>
+  <si>
+    <t>hospital-de-santa-maria.png</t>
+  </si>
+  <si>
+    <t>hopitaux-universitaires-de-strasbourg.jpg</t>
+  </si>
+  <si>
+    <t>hopital-universitaire-necker-enfants-maldes.png</t>
+  </si>
+  <si>
+    <t>helsinki-univeristy-hospital.jpg</t>
+  </si>
+  <si>
+    <t>charite-universitatsmedizin-berlin.jpg</t>
+  </si>
+  <si>
+    <t>haukeland-university-hospital.png</t>
+  </si>
+  <si>
+    <t>childrens-health-ireland-at-temple-street.jpg</t>
   </si>
 </sst>
 </file>
@@ -1269,15 +1395,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0060A8-8459-FC44-9EF8-4FF513B74D7E}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L1" activeCellId="1" sqref="A1:A1048576 L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
@@ -1285,11 +1414,12 @@
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1326,797 +1456,932 @@
       <c r="L1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>282</v>
+      </c>
+      <c r="N1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="F2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G2">
+        <v>56.170313</v>
+      </c>
+      <c r="H2">
+        <v>10.206476</v>
+      </c>
+      <c r="I2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L2" t="s">
+        <v>183</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3">
+        <v>52.374029999999998</v>
+      </c>
+      <c r="H3">
+        <v>4.8896899999999999</v>
+      </c>
+      <c r="I3" t="s">
         <v>164</v>
       </c>
-      <c r="G2">
-        <v>47.799410000000002</v>
-      </c>
-      <c r="H2">
-        <v>13.043990000000001</v>
-      </c>
-      <c r="I2" t="s">
-        <v>165</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="L3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>167</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>168</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>169</v>
-      </c>
-      <c r="E3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3">
-        <v>51.220469999999999</v>
-      </c>
-      <c r="H3">
-        <v>4.4002600000000003</v>
-      </c>
-      <c r="I3" t="s">
-        <v>165</v>
-      </c>
-      <c r="J3" t="s">
-        <v>279</v>
-      </c>
-      <c r="L3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" t="s">
-        <v>174</v>
       </c>
       <c r="F4" t="s">
         <v>150</v>
       </c>
       <c r="G4">
-        <v>51.025171</v>
+        <v>51.220469999999999</v>
       </c>
       <c r="H4">
-        <v>3.7252130000000001</v>
+        <v>4.4002600000000003</v>
       </c>
       <c r="I4" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="J4" t="s">
+        <v>276</v>
       </c>
       <c r="L4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>150</v>
+        <v>67</v>
       </c>
       <c r="G5">
-        <v>50.87959</v>
+        <v>45.404313999999999</v>
       </c>
       <c r="H5">
-        <v>4.7009299999999996</v>
+        <v>11.887473999999999</v>
       </c>
       <c r="I5" t="s">
-        <v>165</v>
-      </c>
-      <c r="J5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K5" t="b">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="L5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>212</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G6">
-        <v>50.072868999999997</v>
+        <v>43.810527</v>
       </c>
       <c r="H6">
-        <v>14.340355000000001</v>
+        <v>11.252438</v>
       </c>
       <c r="I6" t="s">
-        <v>165</v>
-      </c>
-      <c r="K6" t="b">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="L6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>180</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>181</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7">
+        <v>52.524369999999998</v>
+      </c>
+      <c r="H7">
+        <v>13.41053</v>
+      </c>
+      <c r="I7" t="s">
+        <v>164</v>
+      </c>
+      <c r="J7" t="s">
+        <v>143</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8">
+        <v>53.357858</v>
+      </c>
+      <c r="H8">
+        <v>-6.2619809999999996</v>
+      </c>
+      <c r="I8" t="s">
+        <v>164</v>
+      </c>
+      <c r="L8" t="s">
+        <v>207</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9">
+        <v>51.922499999999999</v>
+      </c>
+      <c r="H9">
+        <v>4.4791699999999999</v>
+      </c>
+      <c r="I9" t="s">
+        <v>164</v>
+      </c>
+      <c r="J9" t="s">
+        <v>140</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10">
+        <v>45.477186000000003</v>
+      </c>
+      <c r="H10">
+        <v>9.2303850000000001</v>
+      </c>
+      <c r="I10" t="s">
+        <v>164</v>
+      </c>
+      <c r="L10" t="s">
+        <v>99</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11">
+        <v>41.891930000000002</v>
+      </c>
+      <c r="H11">
+        <v>12.511329999999999</v>
+      </c>
+      <c r="I11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>103</v>
+      </c>
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" t="s">
+        <v>246</v>
+      </c>
+      <c r="G12">
+        <v>60.392989999999998</v>
+      </c>
+      <c r="H12">
+        <v>5.3241500000000004</v>
+      </c>
+      <c r="I12" t="s">
+        <v>164</v>
+      </c>
+      <c r="L12" t="s">
+        <v>247</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13">
+        <v>60.188611000000002</v>
+      </c>
+      <c r="H13">
+        <v>24.905277999999999</v>
+      </c>
+      <c r="I13" t="s">
+        <v>164</v>
+      </c>
+      <c r="L13" t="s">
+        <v>107</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14">
+        <v>48.853409999999997</v>
+      </c>
+      <c r="H14">
+        <v>2.3488000000000002</v>
+      </c>
+      <c r="I14" t="s">
+        <v>164</v>
+      </c>
+      <c r="L14" t="s">
+        <v>94</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15">
+        <v>48.583919999999999</v>
+      </c>
+      <c r="H15">
+        <v>7.7455299999999996</v>
+      </c>
+      <c r="I15" t="s">
+        <v>164</v>
+      </c>
+      <c r="L15" t="s">
+        <v>95</v>
+      </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" t="s">
+        <v>193</v>
+      </c>
+      <c r="E16" t="s">
+        <v>194</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16">
+        <v>45.748460000000001</v>
+      </c>
+      <c r="H16">
+        <v>4.8467099999999999</v>
+      </c>
+      <c r="I16" t="s">
+        <v>164</v>
+      </c>
+      <c r="L16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17">
+        <v>40.416499999999999</v>
+      </c>
+      <c r="H17">
+        <v>-3.7025600000000001</v>
+      </c>
+      <c r="I17" t="s">
+        <v>164</v>
+      </c>
+      <c r="L17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" t="b">
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>268</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" t="s">
+        <v>270</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18">
+        <v>41.38879</v>
+      </c>
+      <c r="H18">
+        <v>2.1589900000000002</v>
+      </c>
+      <c r="I18" t="s">
+        <v>164</v>
+      </c>
+      <c r="L18" t="s">
+        <v>90</v>
+      </c>
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>260</v>
+      </c>
+      <c r="D19" t="s">
+        <v>261</v>
+      </c>
+      <c r="E19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19">
+        <v>38.748446000000001</v>
+      </c>
+      <c r="H19">
+        <v>-9.1606089999999991</v>
+      </c>
+      <c r="I19" t="s">
+        <v>164</v>
+      </c>
+      <c r="L19" t="s">
+        <v>104</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20">
+        <v>59.32938</v>
+      </c>
+      <c r="H20">
+        <v>18.068709999999999</v>
+      </c>
+      <c r="I20" t="s">
+        <v>164</v>
+      </c>
+      <c r="J20" t="s">
+        <v>139</v>
+      </c>
+      <c r="L20" t="s">
+        <v>91</v>
+      </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>230</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" t="s">
+        <v>232</v>
+      </c>
+      <c r="E21" t="s">
+        <v>233</v>
+      </c>
+      <c r="F21" t="s">
+        <v>234</v>
+      </c>
+      <c r="G21">
+        <v>35.901828000000002</v>
+      </c>
+      <c r="H21">
+        <v>14.476744</v>
+      </c>
+      <c r="I21" t="s">
         <v>182</v>
       </c>
-      <c r="G7">
-        <v>56.170313</v>
-      </c>
-      <c r="H7">
-        <v>10.206476</v>
-      </c>
-      <c r="I7" t="s">
-        <v>183</v>
-      </c>
-      <c r="L7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>186</v>
-      </c>
-      <c r="D8" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" t="s">
-        <v>188</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="L21" t="s">
+        <v>235</v>
+      </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>249</v>
+      </c>
+      <c r="D22" t="s">
+        <v>250</v>
+      </c>
+      <c r="E22" t="s">
+        <v>251</v>
+      </c>
+      <c r="F22" t="s">
+        <v>246</v>
+      </c>
+      <c r="G22">
+        <v>59.948599999999999</v>
+      </c>
+      <c r="H22">
+        <v>10.715299999999999</v>
+      </c>
+      <c r="I22" t="s">
+        <v>164</v>
+      </c>
+      <c r="J22" t="s">
+        <v>277</v>
+      </c>
+      <c r="L22" t="s">
+        <v>252</v>
+      </c>
+      <c r="M22" t="b">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>240</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23">
+        <v>51.842500000000001</v>
+      </c>
+      <c r="H23">
+        <v>5.8527800000000001</v>
+      </c>
+      <c r="I23" t="s">
+        <v>164</v>
+      </c>
+      <c r="L23" t="s">
+        <v>93</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>254</v>
+      </c>
+      <c r="D24" t="s">
+        <v>255</v>
+      </c>
+      <c r="E24" t="s">
+        <v>256</v>
+      </c>
+      <c r="F24" t="s">
+        <v>257</v>
+      </c>
+      <c r="G24">
+        <v>53.779949999999999</v>
+      </c>
+      <c r="H24">
+        <v>20.494160000000001</v>
+      </c>
+      <c r="I24" t="s">
         <v>182</v>
       </c>
-      <c r="G8">
-        <v>55.675939999999997</v>
-      </c>
-      <c r="H8">
-        <v>12.565530000000001</v>
-      </c>
-      <c r="I8" t="s">
-        <v>183</v>
-      </c>
-      <c r="L8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9">
-        <v>60.188611000000002</v>
-      </c>
-      <c r="H9">
-        <v>24.905277999999999</v>
-      </c>
-      <c r="I9" t="s">
-        <v>165</v>
-      </c>
-      <c r="L9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>190</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10">
-        <v>48.853409999999997</v>
-      </c>
-      <c r="H10">
-        <v>2.3488000000000002</v>
-      </c>
-      <c r="I10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11">
-        <v>48.583919999999999</v>
-      </c>
-      <c r="H11">
-        <v>7.7455299999999996</v>
-      </c>
-      <c r="I11" t="s">
-        <v>165</v>
-      </c>
-      <c r="L11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12">
-        <v>45.748460000000001</v>
-      </c>
-      <c r="H12">
-        <v>4.8467099999999999</v>
-      </c>
-      <c r="I12" t="s">
-        <v>165</v>
-      </c>
-      <c r="L12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>196</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13">
-        <v>52.524369999999998</v>
-      </c>
-      <c r="H13">
-        <v>13.41053</v>
-      </c>
-      <c r="I13" t="s">
-        <v>165</v>
-      </c>
-      <c r="J13" t="s">
-        <v>143</v>
-      </c>
-      <c r="K13" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>198</v>
-      </c>
-      <c r="D14" t="s">
-        <v>199</v>
-      </c>
-      <c r="E14" t="s">
-        <v>200</v>
-      </c>
-      <c r="F14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14">
-        <v>48.522660000000002</v>
-      </c>
-      <c r="H14">
-        <v>9.0522200000000002</v>
-      </c>
-      <c r="I14" t="s">
-        <v>165</v>
-      </c>
-      <c r="L14" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>202</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E15" t="s">
-        <v>147</v>
-      </c>
-      <c r="F15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15">
-        <v>46.253</v>
-      </c>
-      <c r="H15">
-        <v>20.148240000000001</v>
-      </c>
-      <c r="I15" t="s">
-        <v>165</v>
-      </c>
-      <c r="J15" t="s">
-        <v>144</v>
-      </c>
-      <c r="K15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16">
-        <v>46.072499999999998</v>
-      </c>
-      <c r="H16">
-        <v>18.230830000000001</v>
-      </c>
-      <c r="I16" t="s">
-        <v>165</v>
-      </c>
-      <c r="L16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>203</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>204</v>
-      </c>
-      <c r="D17" t="s">
-        <v>205</v>
-      </c>
-      <c r="E17" t="s">
-        <v>206</v>
-      </c>
-      <c r="F17" t="s">
-        <v>207</v>
-      </c>
-      <c r="G17">
-        <v>53.357858</v>
-      </c>
-      <c r="H17">
-        <v>-6.2619809999999996</v>
-      </c>
-      <c r="I17" t="s">
-        <v>165</v>
-      </c>
-      <c r="L17" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>209</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18">
-        <v>45.404313999999999</v>
-      </c>
-      <c r="H18">
-        <v>11.887473999999999</v>
-      </c>
-      <c r="I18" t="s">
-        <v>165</v>
-      </c>
-      <c r="L18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>210</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>211</v>
-      </c>
-      <c r="D19" t="s">
-        <v>212</v>
-      </c>
-      <c r="E19" t="s">
-        <v>213</v>
-      </c>
-      <c r="F19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19">
-        <v>43.810527</v>
-      </c>
-      <c r="H19">
-        <v>11.252438</v>
-      </c>
-      <c r="I19" t="s">
-        <v>165</v>
-      </c>
-      <c r="L19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>282</v>
-      </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20">
-        <v>45.477186000000003</v>
-      </c>
-      <c r="H20">
-        <v>9.2303850000000001</v>
-      </c>
-      <c r="I20" t="s">
-        <v>165</v>
-      </c>
-      <c r="L20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>215</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21">
-        <v>41.891930000000002</v>
-      </c>
-      <c r="H21">
-        <v>12.511329999999999</v>
-      </c>
-      <c r="I21" t="s">
-        <v>165</v>
-      </c>
-      <c r="J21" t="s">
-        <v>142</v>
-      </c>
-      <c r="K21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" t="s">
-        <v>83</v>
-      </c>
-      <c r="F22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22">
-        <v>45.555954</v>
-      </c>
-      <c r="H22">
-        <v>11.546531999999999</v>
-      </c>
-      <c r="I22" t="s">
-        <v>165</v>
-      </c>
-      <c r="L22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>217</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23">
-        <v>45.603031000000001</v>
-      </c>
-      <c r="H23">
-        <v>9.2587820000000001</v>
-      </c>
-      <c r="I23" t="s">
-        <v>165</v>
-      </c>
-      <c r="J23" t="s">
-        <v>155</v>
-      </c>
-      <c r="K23" t="b">
-        <v>1</v>
-      </c>
-      <c r="L23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="L24" t="s">
+        <v>258</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N24" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>218</v>
       </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24">
-        <v>45.434807999999997</v>
-      </c>
-      <c r="H24">
-        <v>9.1598159999999993</v>
-      </c>
-      <c r="I24" t="s">
-        <v>165</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D25" t="s">
         <v>220</v>
       </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>221</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>222</v>
-      </c>
-      <c r="E25" t="s">
-        <v>223</v>
-      </c>
-      <c r="F25" t="s">
-        <v>224</v>
       </c>
       <c r="G25">
         <v>56.945999999999998</v>
@@ -2125,368 +2390,437 @@
         <v>24.105889999999999</v>
       </c>
       <c r="I25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L25" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="M25" t="b">
+        <v>1</v>
+      </c>
+      <c r="N25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>226</v>
+        <v>184</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>227</v>
+        <v>185</v>
       </c>
       <c r="D26" t="s">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="E26" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
       <c r="F26" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="G26">
-        <v>54.752070000000003</v>
+        <v>55.675939999999997</v>
       </c>
       <c r="H26">
-        <v>25.277787</v>
+        <v>12.565530000000001</v>
       </c>
       <c r="I26" t="s">
+        <v>182</v>
+      </c>
+      <c r="L26" t="s">
+        <v>188</v>
+      </c>
+      <c r="M26" t="b">
+        <v>1</v>
+      </c>
+      <c r="N26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>274</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27">
+        <v>57.707160000000002</v>
+      </c>
+      <c r="H27">
+        <v>11.96679</v>
+      </c>
+      <c r="I27" t="s">
+        <v>164</v>
+      </c>
+      <c r="L27" t="s">
+        <v>88</v>
+      </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28">
+        <v>45.555954</v>
+      </c>
+      <c r="H28">
+        <v>11.546531999999999</v>
+      </c>
+      <c r="I28" t="s">
+        <v>164</v>
+      </c>
+      <c r="L28" t="s">
+        <v>106</v>
+      </c>
+      <c r="M28" t="b">
+        <v>1</v>
+      </c>
+      <c r="N28" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29">
+        <v>45.603031000000001</v>
+      </c>
+      <c r="H29">
+        <v>9.2587820000000001</v>
+      </c>
+      <c r="I29" t="s">
+        <v>164</v>
+      </c>
+      <c r="J29" t="s">
+        <v>155</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>108</v>
+      </c>
+      <c r="M29" t="b">
+        <v>1</v>
+      </c>
+      <c r="N29" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>216</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30">
+        <v>45.434807999999997</v>
+      </c>
+      <c r="H30">
+        <v>9.1598159999999993</v>
+      </c>
+      <c r="I30" t="s">
+        <v>164</v>
+      </c>
+      <c r="L30" t="s">
+        <v>217</v>
+      </c>
+      <c r="M30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N30" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31">
+        <v>46.253</v>
+      </c>
+      <c r="H31">
+        <v>20.148240000000001</v>
+      </c>
+      <c r="I31" t="s">
+        <v>164</v>
+      </c>
+      <c r="J31" t="s">
+        <v>144</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>100</v>
+      </c>
+      <c r="M31" t="b">
+        <v>1</v>
+      </c>
+      <c r="N31" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32">
+        <v>52.090829999999997</v>
+      </c>
+      <c r="H32">
+        <v>5.1222200000000004</v>
+      </c>
+      <c r="I32" t="s">
+        <v>164</v>
+      </c>
+      <c r="J32" t="s">
+        <v>141</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" t="s">
+        <v>241</v>
+      </c>
+      <c r="M32" t="b">
+        <v>1</v>
+      </c>
+      <c r="N32" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>196</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" t="s">
+        <v>198</v>
+      </c>
+      <c r="E33" t="s">
+        <v>199</v>
+      </c>
+      <c r="F33" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33">
+        <v>48.522660000000002</v>
+      </c>
+      <c r="H33">
+        <v>9.0522200000000002</v>
+      </c>
+      <c r="I33" t="s">
+        <v>164</v>
+      </c>
+      <c r="L33" t="s">
+        <v>200</v>
+      </c>
+      <c r="M33" t="b">
+        <v>1</v>
+      </c>
+      <c r="N33" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34">
+        <v>50.072868999999997</v>
+      </c>
+      <c r="H34">
+        <v>14.340355000000001</v>
+      </c>
+      <c r="I34" t="s">
+        <v>164</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
+        <v>105</v>
+      </c>
+      <c r="M34" t="b">
+        <v>1</v>
+      </c>
+      <c r="N34" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>290</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" t="s">
+        <v>162</v>
+      </c>
+      <c r="F35" t="s">
+        <v>163</v>
+      </c>
+      <c r="G35">
+        <v>47.799410000000002</v>
+      </c>
+      <c r="H35">
+        <v>13.043990000000001</v>
+      </c>
+      <c r="I35" t="s">
+        <v>164</v>
+      </c>
+      <c r="L35" t="s">
         <v>165</v>
       </c>
-      <c r="J26" t="s">
+      <c r="M35" t="b">
+        <v>1</v>
+      </c>
+      <c r="N35" t="s">
         <v>281</v>
       </c>
-      <c r="L26" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>232</v>
-      </c>
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D27" t="s">
-        <v>234</v>
-      </c>
-      <c r="E27" t="s">
-        <v>235</v>
-      </c>
-      <c r="F27" t="s">
-        <v>236</v>
-      </c>
-      <c r="G27">
-        <v>35.901828000000002</v>
-      </c>
-      <c r="H27">
-        <v>14.476744</v>
-      </c>
-      <c r="I27" t="s">
-        <v>183</v>
-      </c>
-      <c r="L27" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>238</v>
-      </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>239</v>
-      </c>
-      <c r="D28" t="s">
-        <v>240</v>
-      </c>
-      <c r="E28" t="s">
-        <v>241</v>
-      </c>
-      <c r="F28" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28">
-        <v>52.374029999999998</v>
-      </c>
-      <c r="H28">
-        <v>4.8896899999999999</v>
-      </c>
-      <c r="I28" t="s">
-        <v>165</v>
-      </c>
-      <c r="L28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29">
-        <v>51.922499999999999</v>
-      </c>
-      <c r="H29">
-        <v>4.4791699999999999</v>
-      </c>
-      <c r="I29" t="s">
-        <v>165</v>
-      </c>
-      <c r="J29" t="s">
-        <v>140</v>
-      </c>
-      <c r="K29" t="b">
-        <v>1</v>
-      </c>
-      <c r="L29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>242</v>
-      </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30">
-        <v>51.842500000000001</v>
-      </c>
-      <c r="H30">
-        <v>5.8527800000000001</v>
-      </c>
-      <c r="I30" t="s">
-        <v>165</v>
-      </c>
-      <c r="L30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E31" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31">
-        <v>52.090829999999997</v>
-      </c>
-      <c r="H31">
-        <v>5.1222200000000004</v>
-      </c>
-      <c r="I31" t="s">
-        <v>165</v>
-      </c>
-      <c r="J31" t="s">
-        <v>141</v>
-      </c>
-      <c r="K31" t="b">
-        <v>1</v>
-      </c>
-      <c r="L31" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>244</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>245</v>
-      </c>
-      <c r="D32" t="s">
-        <v>246</v>
-      </c>
-      <c r="E32" t="s">
-        <v>247</v>
-      </c>
-      <c r="F32" t="s">
-        <v>248</v>
-      </c>
-      <c r="G32">
-        <v>60.392989999999998</v>
-      </c>
-      <c r="H32">
-        <v>5.3241500000000004</v>
-      </c>
-      <c r="I32" t="s">
-        <v>165</v>
-      </c>
-      <c r="L32" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>250</v>
-      </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>251</v>
-      </c>
-      <c r="D33" t="s">
-        <v>252</v>
-      </c>
-      <c r="E33" t="s">
-        <v>253</v>
-      </c>
-      <c r="F33" t="s">
-        <v>248</v>
-      </c>
-      <c r="G33">
-        <v>59.948599999999999</v>
-      </c>
-      <c r="H33">
-        <v>10.715299999999999</v>
-      </c>
-      <c r="I33" t="s">
-        <v>165</v>
-      </c>
-      <c r="J33" t="s">
-        <v>280</v>
-      </c>
-      <c r="L33" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>255</v>
-      </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>256</v>
-      </c>
-      <c r="D34" t="s">
-        <v>257</v>
-      </c>
-      <c r="E34" t="s">
-        <v>258</v>
-      </c>
-      <c r="F34" t="s">
-        <v>259</v>
-      </c>
-      <c r="G34">
-        <v>53.779949999999999</v>
-      </c>
-      <c r="H34">
-        <v>20.494160000000001</v>
-      </c>
-      <c r="I34" t="s">
-        <v>183</v>
-      </c>
-      <c r="L34" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>261</v>
-      </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
         <v>262</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>263</v>
       </c>
-      <c r="E35" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35" t="s">
-        <v>77</v>
-      </c>
-      <c r="G35">
-        <v>38.748446000000001</v>
-      </c>
-      <c r="H35">
-        <v>-9.1606089999999991</v>
-      </c>
-      <c r="I35" t="s">
-        <v>165</v>
-      </c>
-      <c r="L35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="E36" t="s">
         <v>264</v>
       </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="F36" t="s">
         <v>265</v>
-      </c>
-      <c r="D36" t="s">
-        <v>266</v>
-      </c>
-      <c r="E36" t="s">
-        <v>267</v>
-      </c>
-      <c r="F36" t="s">
-        <v>268</v>
       </c>
       <c r="G36">
         <v>46.053688999999999</v>
@@ -2495,210 +2829,258 @@
         <v>14.521233000000001</v>
       </c>
       <c r="I36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L36" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+      <c r="M36" t="b">
+        <v>1</v>
+      </c>
+      <c r="N36" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>270</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="F37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37">
+        <v>46.072499999999998</v>
+      </c>
+      <c r="H37">
+        <v>18.230830000000001</v>
+      </c>
+      <c r="I37" t="s">
+        <v>164</v>
+      </c>
+      <c r="L37" t="s">
+        <v>148</v>
+      </c>
+      <c r="M37" t="b">
+        <v>1</v>
+      </c>
+      <c r="N37" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>275</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38">
+        <v>59.847222000000002</v>
+      </c>
+      <c r="H38">
+        <v>17.640277999999999</v>
+      </c>
+      <c r="I38" t="s">
+        <v>164</v>
+      </c>
+      <c r="L38" t="s">
+        <v>98</v>
+      </c>
+      <c r="M38" t="b">
+        <v>1</v>
+      </c>
+      <c r="N38" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" t="s">
+        <v>173</v>
+      </c>
+      <c r="F39" t="s">
+        <v>150</v>
+      </c>
+      <c r="G39">
+        <v>51.025171</v>
+      </c>
+      <c r="H39">
+        <v>3.7252130000000001</v>
+      </c>
+      <c r="I39" t="s">
+        <v>164</v>
+      </c>
+      <c r="L39" t="s">
+        <v>174</v>
+      </c>
+      <c r="M39" t="b">
+        <v>1</v>
+      </c>
+      <c r="N39" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" t="s">
+        <v>154</v>
+      </c>
+      <c r="F40" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40">
+        <v>50.87959</v>
+      </c>
+      <c r="H40">
+        <v>4.7009299999999996</v>
+      </c>
+      <c r="I40" t="s">
+        <v>164</v>
+      </c>
+      <c r="J40" t="s">
+        <v>151</v>
+      </c>
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40" t="s">
+        <v>175</v>
+      </c>
+      <c r="M40" t="b">
+        <v>1</v>
+      </c>
+      <c r="N40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>271</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" t="s">
         <v>59</v>
       </c>
-      <c r="G37">
-        <v>40.416499999999999</v>
-      </c>
-      <c r="H37">
-        <v>-3.7025600000000001</v>
-      </c>
-      <c r="I37" t="s">
-        <v>165</v>
-      </c>
-      <c r="L37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>271</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="G41">
+        <v>41.428083000000001</v>
+      </c>
+      <c r="H41">
+        <v>2.1422780000000001</v>
+      </c>
+      <c r="I41" t="s">
+        <v>164</v>
+      </c>
+      <c r="L41" t="s">
         <v>272</v>
       </c>
-      <c r="D38" t="s">
-        <v>273</v>
-      </c>
-      <c r="E38" t="s">
-        <v>60</v>
-      </c>
-      <c r="F38" t="s">
-        <v>59</v>
-      </c>
-      <c r="G38">
-        <v>41.38879</v>
-      </c>
-      <c r="H38">
-        <v>2.1589900000000002</v>
-      </c>
-      <c r="I38" t="s">
-        <v>165</v>
-      </c>
-      <c r="L38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>274</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39" t="s">
-        <v>59</v>
-      </c>
-      <c r="G39">
-        <v>41.428083000000001</v>
-      </c>
-      <c r="H39">
-        <v>2.1422780000000001</v>
-      </c>
-      <c r="I39" t="s">
-        <v>165</v>
-      </c>
-      <c r="L39" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>276</v>
-      </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" t="s">
-        <v>61</v>
-      </c>
-      <c r="F40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G40">
-        <v>59.32938</v>
-      </c>
-      <c r="H40">
-        <v>18.068709999999999</v>
-      </c>
-      <c r="I40" t="s">
-        <v>165</v>
-      </c>
-      <c r="J40" t="s">
-        <v>139</v>
-      </c>
-      <c r="L40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>277</v>
-      </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E41" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" t="s">
-        <v>57</v>
-      </c>
-      <c r="G41">
-        <v>57.707160000000002</v>
-      </c>
-      <c r="H41">
-        <v>11.96679</v>
-      </c>
-      <c r="I41" t="s">
-        <v>165</v>
-      </c>
-      <c r="L41" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41" t="b">
+        <v>1</v>
+      </c>
+      <c r="N41" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>224</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>225</v>
+      </c>
+      <c r="D42" t="s">
+        <v>226</v>
+      </c>
+      <c r="E42" t="s">
+        <v>227</v>
+      </c>
+      <c r="F42" t="s">
+        <v>228</v>
+      </c>
+      <c r="G42">
+        <v>54.752070000000003</v>
+      </c>
+      <c r="H42">
+        <v>25.277787</v>
+      </c>
+      <c r="I42" t="s">
+        <v>164</v>
+      </c>
+      <c r="J42" t="s">
         <v>278</v>
       </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" t="s">
-        <v>70</v>
-      </c>
-      <c r="F42" t="s">
-        <v>57</v>
-      </c>
-      <c r="G42">
-        <v>59.847222000000002</v>
-      </c>
-      <c r="H42">
-        <v>17.640277999999999</v>
-      </c>
-      <c r="I42" t="s">
-        <v>165</v>
-      </c>
       <c r="L42" t="s">
-        <v>98</v>
+        <v>229</v>
+      </c>
+      <c r="M42" t="b">
+        <v>1</v>
+      </c>
+      <c r="N42" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K25">
-    <sortCondition ref="A2:A25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N42">
+    <sortCondition ref="A2:A42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2903,23 +3285,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6366C3-CBA3-F348-A0A6-D45D62B83798}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
         <v>84</v>
-      </c>
-      <c r="B1" t="s">
-        <v>85</v>
       </c>
       <c r="C1" t="s">
         <v>86</v>
@@ -2927,10 +3309,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>290</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -2938,10 +3320,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
         <v>156</v>
-      </c>
-      <c r="B3" t="s">
-        <v>167</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -2949,10 +3331,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -2960,10 +3342,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -2971,10 +3353,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" t="s">
         <v>105</v>
-      </c>
-      <c r="B6" t="s">
-        <v>177</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -2982,10 +3364,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>97</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -2993,10 +3375,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -3004,10 +3386,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>183</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -3015,10 +3397,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -3026,10 +3408,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>267</v>
       </c>
       <c r="B11" t="s">
-        <v>191</v>
+        <v>89</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -3037,10 +3419,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>268</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>90</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -3048,10 +3430,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>271</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>272</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -3059,10 +3441,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -3070,10 +3452,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
+        <v>94</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -3081,10 +3463,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -3092,10 +3474,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>87</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -3103,10 +3485,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
-        <v>209</v>
+        <v>100</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -3114,10 +3496,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>210</v>
+        <v>148</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -3125,10 +3507,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>202</v>
       </c>
       <c r="B20" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -3136,10 +3518,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>208</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
+        <v>101</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -3147,10 +3529,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="B22" t="s">
-        <v>216</v>
+        <v>96</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -3158,10 +3540,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>279</v>
       </c>
       <c r="B23" t="s">
-        <v>217</v>
+        <v>99</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -3169,10 +3551,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>103</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -3180,10 +3562,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s">
-        <v>220</v>
+        <v>106</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -3191,10 +3573,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="B26" t="s">
-        <v>226</v>
+        <v>108</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -3202,10 +3584,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="B27" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -3213,10 +3595,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>224</v>
       </c>
       <c r="B28" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -3224,10 +3606,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>218</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>223</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -3235,10 +3617,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>230</v>
       </c>
       <c r="B30" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -3246,10 +3628,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -3257,10 +3639,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>249</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>244</v>
+        <v>92</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -3268,10 +3650,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B33" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -3279,10 +3661,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>260</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -3290,10 +3672,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>242</v>
       </c>
       <c r="B35" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -3301,10 +3683,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="B36" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -3312,10 +3694,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>253</v>
       </c>
       <c r="B37" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -3323,10 +3705,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>259</v>
       </c>
       <c r="B38" t="s">
-        <v>271</v>
+        <v>104</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -3334,10 +3716,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B39" t="s">
-        <v>274</v>
+        <v>91</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -3345,10 +3727,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>274</v>
       </c>
       <c r="B40" t="s">
-        <v>276</v>
+        <v>88</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -3356,10 +3738,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>275</v>
       </c>
       <c r="B41" t="s">
-        <v>277</v>
+        <v>98</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -3367,16 +3749,19 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>298</v>
       </c>
       <c r="B42" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C42">
+    <sortCondition ref="B2:B42"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>